<commit_message>
session transfer through subbot
</commit_message>
<xml_diff>
--- a/TransferSessionInvariable/Invoice_Sample.xlsx
+++ b/TransferSessionInvariable/Invoice_Sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46D48AE-F571-4C8E-9CB8-C7D012AD19E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B2657B-49DB-4B2D-ACA2-74DC9AD72E6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">S no </t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Organic Retail</t>
+  </si>
+  <si>
+    <t>LiterRet Inc</t>
+  </si>
+  <si>
+    <t>$ 234</t>
   </si>
 </sst>
 </file>
@@ -81,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -162,17 +168,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +545,17 @@
       </c>
       <c r="D4" s="1"/>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>